<commit_message>
Expanded Chase module features
</commit_message>
<xml_diff>
--- a/Documents/LED_StarLiteUP_Instruction.xlsx
+++ b/Documents/LED_StarLiteUP_Instruction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Starlite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFBBDF5-A166-4EB3-9612-AA26D3D34394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB855624-FE9E-41BA-9DB7-E94CE71CBD58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28116" yWindow="1272" windowWidth="15096" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>Red</t>
   </si>
@@ -304,6 +304,25 @@
   </si>
   <si>
     <t>Uses random color palette in Instruction 9</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Offset size [25:20] </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>For backwards compatability, an offset size of 0 = 1. All others = number entered</t>
   </si>
 </sst>
 </file>
@@ -721,6 +740,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -774,54 +841,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,16 +1396,16 @@
       <c r="E19" s="40"/>
     </row>
     <row r="20" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="70">
+      <c r="B20" s="86">
         <v>3</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="70" t="s">
+      <c r="D20" s="86" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="43" t="s">
@@ -1394,19 +1413,19 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="68"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="71"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="54" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="69"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="72"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="44"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1429,39 +1448,41 @@
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="70">
+      <c r="B24" s="86">
         <v>5</v>
       </c>
-      <c r="C24" s="76"/>
+      <c r="C24" s="86" t="s">
+        <v>74</v>
+      </c>
       <c r="D24" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="76"/>
+      <c r="E24" s="92"/>
       <c r="F24" s="2"/>
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="83"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="77"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
       <c r="D25" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="77"/>
+      <c r="E25" s="93"/>
       <c r="F25" s="2"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="78"/>
+      <c r="A26" s="100"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="78"/>
+      <c r="E26" s="94"/>
       <c r="F26" s="2"/>
       <c r="G26"/>
     </row>
@@ -1479,10 +1500,10 @@
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="79">
+      <c r="B28" s="95">
         <v>7</v>
       </c>
       <c r="C28" s="57" t="s">
@@ -1491,31 +1512,31 @@
       <c r="D28" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="76"/>
+      <c r="E28" s="92"/>
       <c r="F28" s="2"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="83"/>
-      <c r="B29" s="80"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="96"/>
       <c r="C29" s="58" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="77"/>
+      <c r="E29" s="93"/>
       <c r="F29" s="2"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
-      <c r="B30" s="81"/>
+      <c r="A30" s="100"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="59" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="62"/>
-      <c r="E30" s="78"/>
+      <c r="E30" s="94"/>
       <c r="F30" s="2"/>
       <c r="G30"/>
     </row>
@@ -1554,55 +1575,55 @@
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="85">
+      <c r="B33" s="67">
         <v>10</v>
       </c>
-      <c r="C33" s="87"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="89" t="s">
+      <c r="E33" s="71" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="100"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="88"/>
+      <c r="A34" s="82"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="70"/>
       <c r="D34" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="90"/>
+      <c r="E34" s="72"/>
       <c r="F34" s="2"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="93">
+      <c r="B35" s="75">
         <v>11</v>
       </c>
-      <c r="C35" s="95"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="97"/>
+      <c r="E35" s="79"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="92"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="96"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="78"/>
       <c r="D36" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="98"/>
+      <c r="E36" s="80"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1752,8 +1773,12 @@
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="24"/>
-      <c r="B49" s="15"/>
+      <c r="A49" s="24">
+        <v>2</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="C49" s="5"/>
       <c r="D49" s="13"/>
       <c r="E49" s="23"/>
@@ -1821,14 +1846,6 @@
     <row r="57" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A33:A34"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="C20:C22"/>
@@ -1840,6 +1857,14 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>